<commit_message>
Integrate song count into song list, improve song title matching
</commit_message>
<xml_diff>
--- a/rcc-song-summary/RCC Song List Template.xlsx
+++ b/rcc-song-summary/RCC Song List Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drump\Code\rcc-utils\rcc-song-summary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507D481A-1055-4D89-85AE-71B45EDC7ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3498251E-A780-48E3-9A10-E650CD708892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Folder</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>Copyright</t>
+  </si>
+  <si>
+    <t>Times Sung</t>
   </si>
 </sst>
 </file>
@@ -92,13 +95,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFCCCC"/>
         </patternFill>
       </fill>
@@ -107,6 +103,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFCC99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -448,11 +451,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,10 +464,11 @@
     <col min="2" max="2" width="43" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="89.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="89.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -478,22 +482,25 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>"Bethel"</formula>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"Hillsong"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Elevation"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"Hillsong"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"Bethel"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
More word count improvements
</commit_message>
<xml_diff>
--- a/rcc-song-summary/RCC Song List Template.xlsx
+++ b/rcc-song-summary/RCC Song List Template.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drump\Code\rcc-utils\rcc-song-summary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D37A9B-413B-42A8-811D-8680050CC8D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4184E5-782F-44B6-8AFC-BB77383F2548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Song List" sheetId="1" r:id="rId1"/>
+    <sheet name="Word Counts" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -99,28 +100,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -482,9 +462,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1:G1048576"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,18 +509,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
       <formula>"Hillsong"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
       <formula>"Elevation"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
       <formula>"Bethel"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{3150816C-8037-496A-9FB4-486F8051FE93}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -550,7 +544,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -560,5 +554,320 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{3150816C-8037-496A-9FB4-486F8051FE93}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E1:E1048576</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8D8D5D1-1EE1-475B-A367-FA30679BC5FC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="K1" sqref="K1:K1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="11" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="dataBar" priority="10">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D7EF2651-0F5D-41F4-96BA-BDF35E4584F2}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="dataBar" priority="9">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{E90A355C-6641-475C-84B3-94D559AB4C7A}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="dataBar" priority="8">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{5B3E672E-1684-423B-8B23-4109741CF47D}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="dataBar" priority="7">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{B748EB77-6283-44EA-AA88-D5CDD8647CB1}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="dataBar" priority="6">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{1BE3B903-D108-4792-B587-66850DA8B63F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="dataBar" priority="5">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{470FE130-27ED-422E-A48B-64FB7A46AE31}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H1:H1048576">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2318D484-0E5B-4900-B834-32AACDF94DAE}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{731CBD3C-409F-4B4F-9B54-C10845ACB4E9}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1:J1048576">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{58AE70D2-8480-4257-BB44-F716EFC241AC}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K1:K1048576">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{BE5FAF0E-8816-469E-88E4-0BE377DCF115}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{D7EF2651-0F5D-41F4-96BA-BDF35E4584F2}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>B1:B1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{E90A355C-6641-475C-84B3-94D559AB4C7A}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C1:C1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{5B3E672E-1684-423B-8B23-4109741CF47D}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D1:D1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{B748EB77-6283-44EA-AA88-D5CDD8647CB1}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E1:E1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{1BE3B903-D108-4792-B587-66850DA8B63F}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F1:F1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{470FE130-27ED-422E-A48B-64FB7A46AE31}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G1:G1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{2318D484-0E5B-4900-B834-32AACDF94DAE}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H1:H1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{731CBD3C-409F-4B4F-9B54-C10845ACB4E9}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I1:I1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{58AE70D2-8480-4257-BB44-F716EFC241AC}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>J1:J1048576</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{BE5FAF0E-8816-469E-88E4-0BE377DCF115}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>K1:K1048576</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>